<commit_message>
Portfolio Investment data preparation (date formatting, additional metrics, removed second column layer)
</commit_message>
<xml_diff>
--- a/data/inputs.xlsx
+++ b/data/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuinvest-my.sharepoint.com/personal/felix_vogt_tuinvest_de/Documents/04_MSMIF/TUIC-PortfolioModel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{AFB54F55-06F0-5F48-8724-3AE54FA80DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F836DFEE-2E3F-D442-B392-F4F31BA379AC}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{AFB54F55-06F0-5F48-8724-3AE54FA80DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76D5CB19-BD07-F545-AF00-20E819385D1F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9CF08E29-48AC-0A47-82FF-8C3444418925}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{9CF08E29-48AC-0A47-82FF-8C3444418925}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Equity</t>
-  </si>
-  <si>
-    <t>Ticker</t>
-  </si>
-  <si>
-    <t>Buy-in-date</t>
-  </si>
-  <si>
-    <t>Buy-in-amount</t>
-  </si>
-  <si>
-    <t>Exit-date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>PayPal</t>
   </si>
@@ -78,6 +63,24 @@
   </si>
   <si>
     <t>01.05.2023</t>
+  </si>
+  <si>
+    <t>equity</t>
+  </si>
+  <si>
+    <t>ticker</t>
+  </si>
+  <si>
+    <t>buy_in_date</t>
+  </si>
+  <si>
+    <t>shares</t>
+  </si>
+  <si>
+    <t>buy_in_amount</t>
+  </si>
+  <si>
+    <t>exit_date</t>
   </si>
 </sst>
 </file>
@@ -449,75 +452,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0EE013-C17D-F34F-B9F7-B69AA393D8C9}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="5" width="15.83203125" customWidth="1"/>
+    <col min="3" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
         <v>1200</v>
       </c>
     </row>

</xml_diff>